<commit_message>
paper mexico simulation update
</commit_message>
<xml_diff>
--- a/Accounting for Mexican Business Cycles/DSGE/data.xlsx
+++ b/Accounting for Mexican Business Cycles/DSGE/data.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+  <si>
+    <t>quarter</t>
+  </si>
   <si>
     <t>ee</t>
   </si>
@@ -348,7 +351,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11.0"/>
@@ -378,8 +383,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -400,1193 +407,1520 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" t="n" s="2">
+        <v>34335.0</v>
+      </c>
+      <c r="C2" t="n">
         <v>-0.14590742480700536</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.019088025247304338</v>
+      <c r="D2" t="n">
+        <v>-1.3671484769279374</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n" s="2">
+        <v>34425.0</v>
+      </c>
+      <c r="C3" t="n">
         <v>-0.10328867466050162</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.028869978844341983</v>
+      <c r="D3" t="n">
+        <v>-0.4929098731022208</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" t="n" s="2">
+        <v>34516.0</v>
+      </c>
+      <c r="C4" t="n">
         <v>-0.08644507634405119</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.027856206438867798</v>
+      <c r="D4" t="n">
+        <v>-0.6851447002295785</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" t="n" s="2">
+        <v>34608.0</v>
+      </c>
+      <c r="C5" t="n">
         <v>-0.037050810741683815</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.03406450700909171</v>
+      <c r="D5" t="n">
+        <v>-0.13529048065006322</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B6" t="n" s="2">
+        <v>34700.0</v>
+      </c>
+      <c r="C6" t="n">
         <v>0.48364248216412564</v>
       </c>
-      <c r="C6" t="n">
-        <v>-0.01649258604314559</v>
+      <c r="D6" t="n">
+        <v>-5.233570281437494</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="n">
+        <v>8</v>
+      </c>
+      <c r="B7" t="n" s="2">
+        <v>34790.0</v>
+      </c>
+      <c r="C7" t="n">
         <v>0.314754743117841</v>
       </c>
-      <c r="C7" t="n">
-        <v>-0.0662609643541718</v>
+      <c r="D7" t="n">
+        <v>-10.213920641795227</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="n">
+        <v>9</v>
+      </c>
+      <c r="B8" t="n" s="2">
+        <v>34881.0</v>
+      </c>
+      <c r="C8" t="n">
         <v>0.23081641029180844</v>
       </c>
-      <c r="C8" t="n">
-        <v>-0.05609386926067588</v>
+      <c r="D8" t="n">
+        <v>-9.152043857589653</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+      <c r="B9" t="n" s="2">
+        <v>34973.0</v>
+      </c>
+      <c r="C9" t="n">
         <v>0.3652960748781917</v>
       </c>
-      <c r="C9" t="n">
-        <v>-0.049767159358166634</v>
+      <c r="D9" t="n">
+        <v>-8.420045260842102</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="n">
+        <v>11</v>
+      </c>
+      <c r="B10" t="n" s="2">
+        <v>35065.0</v>
+      </c>
+      <c r="C10" t="n">
         <v>0.28090858226221127</v>
       </c>
-      <c r="C10" t="n">
-        <v>-0.033746491814110394</v>
+      <c r="D10" t="n">
+        <v>-6.662515907597566</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="n">
+        <v>12</v>
+      </c>
+      <c r="B11" t="n" s="2">
+        <v>35156.0</v>
+      </c>
+      <c r="C11" t="n">
         <v>0.20014401952836036</v>
       </c>
-      <c r="C11" t="n">
-        <v>-0.03178352993414568</v>
+      <c r="D11" t="n">
+        <v>-6.255757915178961</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="n">
+        <v>13</v>
+      </c>
+      <c r="B12" t="n" s="2">
+        <v>35247.0</v>
+      </c>
+      <c r="C12" t="n">
         <v>0.16442936589443535</v>
       </c>
-      <c r="C12" t="n">
-        <v>-0.026653487308614734</v>
+      <c r="D12" t="n">
+        <v>-5.48053758511724</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="n">
+        <v>14</v>
+      </c>
+      <c r="B13" t="n" s="2">
+        <v>35339.0</v>
+      </c>
+      <c r="C13" t="n">
         <v>0.1557498390612988</v>
       </c>
-      <c r="C13" t="n">
-        <v>-0.010155731281000311</v>
+      <c r="D13" t="n">
+        <v>-3.522023064878965</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="n">
+        <v>15</v>
+      </c>
+      <c r="B14" t="n" s="2">
+        <v>35431.0</v>
+      </c>
+      <c r="C14" t="n">
         <v>0.07970618630015003</v>
       </c>
-      <c r="C14" t="n">
-        <v>-0.014906345711327394</v>
+      <c r="D14" t="n">
+        <v>-3.648719996541061</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="n">
+        <v>16</v>
+      </c>
+      <c r="B15" t="n" s="2">
+        <v>35521.0</v>
+      </c>
+      <c r="C15" t="n">
         <v>0.05312260850428108</v>
       </c>
-      <c r="C15" t="n">
-        <v>-0.005353170276229096</v>
+      <c r="D15" t="n">
+        <v>-2.3129443370468294</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="n">
+        <v>17</v>
+      </c>
+      <c r="B16" t="n" s="2">
+        <v>35612.0</v>
+      </c>
+      <c r="C16" t="n">
         <v>0.00801361137218426</v>
       </c>
-      <c r="C16" t="n">
-        <v>0.004038896449757201</v>
+      <c r="D16" t="n">
+        <v>-0.9696495797369309</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="n">
+        <v>18</v>
+      </c>
+      <c r="B17" t="n" s="2">
+        <v>35704.0</v>
+      </c>
+      <c r="C17" t="n">
         <v>0.005153404823387442</v>
       </c>
-      <c r="C17" t="n">
-        <v>0.017746471685023905</v>
+      <c r="D17" t="n">
+        <v>0.8200277881991624</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="n">
+        <v>19</v>
+      </c>
+      <c r="B18" t="n" s="2">
+        <v>35796.0</v>
+      </c>
+      <c r="C18" t="n">
         <v>-0.014407236956754832</v>
       </c>
-      <c r="C18" t="n">
-        <v>0.018207560817369052</v>
+      <c r="D18" t="n">
+        <v>1.291342527539996</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="n">
+        <v>20</v>
+      </c>
+      <c r="B19" t="n" s="2">
+        <v>35886.0</v>
+      </c>
+      <c r="C19" t="n">
         <v>-0.012935107252093236</v>
       </c>
-      <c r="C19" t="n">
-        <v>0.015665945928193016</v>
+      <c r="D19" t="n">
+        <v>1.4612362229053488</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="n">
+        <v>21</v>
+      </c>
+      <c r="B20" t="n" s="2">
+        <v>35977.0</v>
+      </c>
+      <c r="C20" t="n">
         <v>0.04532988491200296</v>
       </c>
-      <c r="C20" t="n">
-        <v>0.012996978527813263</v>
+      <c r="D20" t="n">
+        <v>1.6109453743570867</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="n">
+        <v>22</v>
+      </c>
+      <c r="B21" t="n" s="2">
+        <v>36069.0</v>
+      </c>
+      <c r="C21" t="n">
         <v>0.07163114489565814</v>
       </c>
-      <c r="C21" t="n">
-        <v>0.006330050264528441</v>
+      <c r="D21" t="n">
+        <v>1.3480896173764023</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="n">
+        <v>23</v>
+      </c>
+      <c r="B22" t="n" s="2">
+        <v>36161.0</v>
+      </c>
+      <c r="C22" t="n">
         <v>0.003590176222406649</v>
       </c>
-      <c r="C22" t="n">
-        <v>0.004642180793858024</v>
+      <c r="D22" t="n">
+        <v>1.5658636993238773</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="n">
+        <v>24</v>
+      </c>
+      <c r="B23" t="n" s="2">
+        <v>36251.0</v>
+      </c>
+      <c r="C23" t="n">
         <v>-0.07259352206820202</v>
       </c>
-      <c r="C23" t="n">
-        <v>0.0025327335625022034</v>
+      <c r="D23" t="n">
+        <v>1.7200923748204033</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="n">
+        <v>25</v>
+      </c>
+      <c r="B24" t="n" s="2">
+        <v>36342.0</v>
+      </c>
+      <c r="C24" t="n">
         <v>-0.09265592300405856</v>
       </c>
-      <c r="C24" t="n">
-        <v>0.0027665778755094766</v>
+      <c r="D24" t="n">
+        <v>2.083441120620577</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" t="n">
+        <v>26</v>
+      </c>
+      <c r="B25" t="n" s="2">
+        <v>36434.0</v>
+      </c>
+      <c r="C25" t="n">
         <v>-0.09669941529803117</v>
       </c>
-      <c r="C25" t="n">
-        <v>0.00648643611093078</v>
+      <c r="D25" t="n">
+        <v>2.766519016627633</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" t="n">
+        <v>27</v>
+      </c>
+      <c r="B26" t="n" s="2">
+        <v>36526.0</v>
+      </c>
+      <c r="C26" t="n">
         <v>-0.12546088205336892</v>
       </c>
-      <c r="C26" t="n">
-        <v>0.017324627485026858</v>
+      <c r="D26" t="n">
+        <v>4.129067737682313</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" t="n">
+        <v>28</v>
+      </c>
+      <c r="B27" t="n" s="2">
+        <v>36617.0</v>
+      </c>
+      <c r="C27" t="n">
         <v>-0.12295964328634479</v>
       </c>
-      <c r="C27" t="n">
-        <v>0.02734743101368859</v>
+      <c r="D27" t="n">
+        <v>5.374630340845954</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" t="n">
+        <v>29</v>
+      </c>
+      <c r="B28" t="n" s="2">
+        <v>36708.0</v>
+      </c>
+      <c r="C28" t="n">
         <v>-0.15438779325827734</v>
       </c>
-      <c r="C28" t="n">
-        <v>0.03416135949075496</v>
+      <c r="D28" t="n">
+        <v>6.261856050191916</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="n">
+        <v>30</v>
+      </c>
+      <c r="B29" t="n" s="2">
+        <v>36800.0</v>
+      </c>
+      <c r="C29" t="n">
         <v>-0.1632255229177999</v>
       </c>
-      <c r="C29" t="n">
-        <v>0.023562348180568727</v>
+      <c r="D29" t="n">
+        <v>5.370045551282843</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="n">
+        <v>31</v>
+      </c>
+      <c r="B30" t="n" s="2">
+        <v>36892.0</v>
+      </c>
+      <c r="C30" t="n">
         <v>-0.15443875297068665</v>
       </c>
-      <c r="C30" t="n">
-        <v>0.019164643263070054</v>
+      <c r="D30" t="n">
+        <v>5.0624657062089184</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" t="n">
+        <v>32</v>
+      </c>
+      <c r="B31" t="n" s="2">
+        <v>36982.0</v>
+      </c>
+      <c r="C31" t="n">
         <v>-0.20861549703800897</v>
       </c>
-      <c r="C31" t="n">
-        <v>0.009592582609505365</v>
+      <c r="D31" t="n">
+        <v>4.204865192952134</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" t="n">
+        <v>33</v>
+      </c>
+      <c r="B32" t="n" s="2">
+        <v>37073.0</v>
+      </c>
+      <c r="C32" t="n">
         <v>-0.20865049920121803</v>
       </c>
-      <c r="C32" t="n">
-        <v>0.006549335566723331</v>
+      <c r="D32" t="n">
+        <v>3.9720736272592205</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" t="n">
+        <v>34</v>
+      </c>
+      <c r="B33" t="n" s="2">
+        <v>37165.0</v>
+      </c>
+      <c r="C33" t="n">
         <v>-0.22249690695890612</v>
       </c>
-      <c r="C33" t="n">
-        <v>-0.0048359193786809505</v>
+      <c r="D33" t="n">
+        <v>2.8821210752639104</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" t="n">
+        <v>35</v>
+      </c>
+      <c r="B34" t="n" s="2">
+        <v>37257.0</v>
+      </c>
+      <c r="C34" t="n">
         <v>-0.24634971309103315</v>
       </c>
-      <c r="C34" t="n">
-        <v>-0.014708712560781685</v>
+      <c r="D34" t="n">
+        <v>1.925976054506684</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" t="n">
+        <v>36</v>
+      </c>
+      <c r="B35" t="n" s="2">
+        <v>37347.0</v>
+      </c>
+      <c r="C35" t="n">
         <v>-0.21152315483185624</v>
       </c>
-      <c r="C35" t="n">
-        <v>-0.01229571141896659</v>
+      <c r="D35" t="n">
+        <v>2.1861911270347534</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" t="n">
+        <v>37</v>
+      </c>
+      <c r="B36" t="n" s="2">
+        <v>37438.0</v>
+      </c>
+      <c r="C36" t="n">
         <v>-0.1775735542223873</v>
       </c>
-      <c r="C36" t="n">
-        <v>-0.010378040375007044</v>
+      <c r="D36" t="n">
+        <v>2.3889538621226336</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" t="n">
+        <v>38</v>
+      </c>
+      <c r="B37" t="n" s="2">
+        <v>37530.0</v>
+      </c>
+      <c r="C37" t="n">
         <v>-0.16693217081073952</v>
       </c>
-      <c r="C37" t="n">
-        <v>-0.012147818304386321</v>
+      <c r="D37" t="n">
+        <v>2.218583901709259</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" t="n">
+        <v>39</v>
+      </c>
+      <c r="B38" t="n" s="2">
+        <v>37622.0</v>
+      </c>
+      <c r="C38" t="n">
         <v>-0.10553538615145253</v>
       </c>
-      <c r="C38" t="n">
-        <v>-0.015149734956358149</v>
+      <c r="D38" t="n">
+        <v>1.923495172833789</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" t="n">
+        <v>40</v>
+      </c>
+      <c r="B39" t="n" s="2">
+        <v>37712.0</v>
+      </c>
+      <c r="C39" t="n">
         <v>-0.1262607507099407</v>
       </c>
-      <c r="C39" t="n">
-        <v>-0.018210452648130305</v>
+      <c r="D39" t="n">
+        <v>1.6231451070952474</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" t="n">
+        <v>41</v>
+      </c>
+      <c r="B40" t="n" s="2">
+        <v>37803.0</v>
+      </c>
+      <c r="C40" t="n">
         <v>-0.10468490899452154</v>
       </c>
-      <c r="C40" t="n">
-        <v>-0.022260506788282952</v>
+      <c r="D40" t="n">
+        <v>1.2256569685213492</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" t="n">
+        <v>42</v>
+      </c>
+      <c r="B41" t="n" s="2">
+        <v>37895.0</v>
+      </c>
+      <c r="C41" t="n">
         <v>-0.06565245531125385</v>
       </c>
-      <c r="C41" t="n">
-        <v>-0.018117423469109814</v>
+      <c r="D41" t="n">
+        <v>1.6493167994772406</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" t="n">
+        <v>43</v>
+      </c>
+      <c r="B42" t="n" s="2">
+        <v>37987.0</v>
+      </c>
+      <c r="C42" t="n">
         <v>-0.0827268203268664</v>
       </c>
-      <c r="C42" t="n">
-        <v>-0.009530914782648805</v>
+      <c r="D42" t="n">
+        <v>2.517800760680089</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" t="n">
+        <v>44</v>
+      </c>
+      <c r="B43" t="n" s="2">
+        <v>38078.0</v>
+      </c>
+      <c r="C43" t="n">
         <v>-0.04901231494964253</v>
       </c>
-      <c r="C43" t="n">
-        <v>-0.001728040028698319</v>
+      <c r="D43" t="n">
+        <v>3.30591795310351</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" t="n">
+        <v>45</v>
+      </c>
+      <c r="B44" t="n" s="2">
+        <v>38169.0</v>
+      </c>
+      <c r="C44" t="n">
         <v>-0.04683402706622841</v>
       </c>
-      <c r="C44" t="n">
-        <v>-0.007013677245610163</v>
+      <c r="D44" t="n">
+        <v>2.780099921692525</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" t="n">
+        <v>46</v>
+      </c>
+      <c r="B45" t="n" s="2">
+        <v>38261.0</v>
+      </c>
+      <c r="C45" t="n">
         <v>-0.05730587141917476</v>
       </c>
-      <c r="C45" t="n">
-        <v>-5.357869868904443E-4</v>
+      <c r="D45" t="n">
+        <v>3.4223619573742425</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" t="n">
+        <v>47</v>
+      </c>
+      <c r="B46" t="n" s="2">
+        <v>38353.0</v>
+      </c>
+      <c r="C46" t="n">
         <v>-0.06546619893019068</v>
       </c>
-      <c r="C46" t="n">
-        <v>-0.003079258953872033</v>
+      <c r="D46" t="n">
+        <v>3.150588081465955</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" t="n">
+        <v>48</v>
+      </c>
+      <c r="B47" t="n" s="2">
+        <v>38443.0</v>
+      </c>
+      <c r="C47" t="n">
         <v>-0.0841530881068776</v>
       </c>
-      <c r="C47" t="n">
-        <v>-0.005029946872923139</v>
+      <c r="D47" t="n">
+        <v>2.922532426094193</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" t="n">
+        <v>49</v>
+      </c>
+      <c r="B48" t="n" s="2">
+        <v>38534.0</v>
+      </c>
+      <c r="C48" t="n">
         <v>-0.10415689546647999</v>
       </c>
-      <c r="C48" t="n">
-        <v>-0.0035459648339014258</v>
+      <c r="D48" t="n">
+        <v>3.018530633351979</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" t="n">
+        <v>50</v>
+      </c>
+      <c r="B49" t="n" s="2">
+        <v>38626.0</v>
+      </c>
+      <c r="C49" t="n">
         <v>-0.11466488608236958</v>
       </c>
-      <c r="C49" t="n">
-        <v>0.005968728195286568</v>
+      <c r="D49" t="n">
+        <v>3.8940194858483324</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" t="n">
+        <v>51</v>
+      </c>
+      <c r="B50" t="n" s="2">
+        <v>38718.0</v>
+      </c>
+      <c r="C50" t="n">
         <v>-0.12618597540381538</v>
       </c>
-      <c r="C50" t="n">
-        <v>0.01545049801185321</v>
+      <c r="D50" t="n">
+        <v>4.738246619901432</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" t="n">
+        <v>52</v>
+      </c>
+      <c r="B51" t="n" s="2">
+        <v>38808.0</v>
+      </c>
+      <c r="C51" t="n">
         <v>-0.05860911424496451</v>
       </c>
-      <c r="C51" t="n">
-        <v>0.019022480515139013</v>
+      <c r="D51" t="n">
+        <v>4.9595097275551225</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" t="n">
+        <v>53</v>
+      </c>
+      <c r="B52" t="n" s="2">
+        <v>38899.0</v>
+      </c>
+      <c r="C52" t="n">
         <v>-0.08039744054187636</v>
       </c>
-      <c r="C52" t="n">
-        <v>0.01865053709010772</v>
+      <c r="D52" t="n">
+        <v>4.751344705540639</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53" t="n">
+        <v>54</v>
+      </c>
+      <c r="B53" t="n" s="2">
+        <v>38991.0</v>
+      </c>
+      <c r="C53" t="n">
         <v>-0.10155169185532531</v>
       </c>
-      <c r="C53" t="n">
-        <v>0.017772645623054424</v>
+      <c r="D53" t="n">
+        <v>4.455688005755221</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>54</v>
-      </c>
-      <c r="B54" t="n">
+        <v>55</v>
+      </c>
+      <c r="B54" t="n" s="2">
+        <v>39083.0</v>
+      </c>
+      <c r="C54" t="n">
         <v>-0.09236445839553076</v>
       </c>
-      <c r="C54" t="n">
-        <v>0.02154037754613855</v>
+      <c r="D54" t="n">
+        <v>4.587001093250009</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>55</v>
-      </c>
-      <c r="B55" t="n">
+        <v>56</v>
+      </c>
+      <c r="B55" t="n" s="2">
+        <v>39173.0</v>
+      </c>
+      <c r="C55" t="n">
         <v>-0.08026065788392489</v>
       </c>
-      <c r="C55" t="n">
-        <v>0.024996677704058282</v>
+      <c r="D55" t="n">
+        <v>4.64999356468212</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" t="n">
+        <v>57</v>
+      </c>
+      <c r="B56" t="n" s="2">
+        <v>39264.0</v>
+      </c>
+      <c r="C56" t="n">
         <v>-0.06941795325403399</v>
       </c>
-      <c r="C56" t="n">
-        <v>0.02710933399941171</v>
+      <c r="D56" t="n">
+        <v>4.543205596094602</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57" t="n">
+        <v>58</v>
+      </c>
+      <c r="B57" t="n" s="2">
+        <v>39356.0</v>
+      </c>
+      <c r="C57" t="n">
         <v>-0.07104189033847452</v>
       </c>
-      <c r="C57" t="n">
-        <v>0.02700821315640145</v>
+      <c r="D57" t="n">
+        <v>4.182947538048154</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58" t="n">
+        <v>59</v>
+      </c>
+      <c r="B58" t="n" s="2">
+        <v>39448.0</v>
+      </c>
+      <c r="C58" t="n">
         <v>-0.06503388979913338</v>
       </c>
-      <c r="C58" t="n">
-        <v>0.021709714557173118</v>
+      <c r="D58" t="n">
+        <v>3.275877340272082</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" t="n">
+        <v>60</v>
+      </c>
+      <c r="B59" t="n" s="2">
+        <v>39539.0</v>
+      </c>
+      <c r="C59" t="n">
         <v>-0.08196228324508315</v>
       </c>
-      <c r="C59" t="n">
-        <v>0.024572599139759312</v>
+      <c r="D59" t="n">
+        <v>3.1645771214073193</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" t="n">
+        <v>61</v>
+      </c>
+      <c r="B60" t="n" s="2">
+        <v>39630.0</v>
+      </c>
+      <c r="C60" t="n">
         <v>-0.10405506554338417</v>
       </c>
-      <c r="C60" t="n">
-        <v>0.024371661404575775</v>
+      <c r="D60" t="n">
+        <v>2.734589213492278</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" t="n">
+        <v>62</v>
+      </c>
+      <c r="B61" t="n" s="2">
+        <v>39722.0</v>
+      </c>
+      <c r="C61" t="n">
         <v>0.04636302177577112</v>
       </c>
-      <c r="C61" t="n">
-        <v>0.009311543881154651</v>
+      <c r="D61" t="n">
+        <v>0.8159765389239126</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>62</v>
-      </c>
-      <c r="B62" t="n">
+        <v>63</v>
+      </c>
+      <c r="B62" t="n" s="2">
+        <v>39814.0</v>
+      </c>
+      <c r="C62" t="n">
         <v>0.12435161915950244</v>
       </c>
-      <c r="C62" t="n">
-        <v>-0.0357077412117531</v>
+      <c r="D62" t="n">
+        <v>-4.090137782141667</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" t="n">
+        <v>64</v>
+      </c>
+      <c r="B63" t="n" s="2">
+        <v>39904.0</v>
+      </c>
+      <c r="C63" t="n">
         <v>0.057795068639788116</v>
       </c>
-      <c r="C63" t="n">
-        <v>-0.052806735702504506</v>
+      <c r="D63" t="n">
+        <v>-6.184104062766593</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64" t="n">
+        <v>65</v>
+      </c>
+      <c r="B64" t="n" s="2">
+        <v>39995.0</v>
+      </c>
+      <c r="C64" t="n">
         <v>0.06697436094858245</v>
       </c>
-      <c r="C64" t="n">
-        <v>-0.03193420587482834</v>
+      <c r="D64" t="n">
+        <v>-4.4513267953753655</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>65</v>
-      </c>
-      <c r="B65" t="n">
+        <v>66</v>
+      </c>
+      <c r="B65" t="n" s="2">
+        <v>40087.0</v>
+      </c>
+      <c r="C65" t="n">
         <v>0.055513274242024346</v>
       </c>
-      <c r="C65" t="n">
-        <v>-0.02486254376638476</v>
+      <c r="D65" t="n">
+        <v>-4.062873468767769</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>66</v>
-      </c>
-      <c r="B66" t="n">
+        <v>67</v>
+      </c>
+      <c r="B66" t="n" s="2">
+        <v>40179.0</v>
+      </c>
+      <c r="C66" t="n">
         <v>0.010317593103680966</v>
       </c>
-      <c r="C66" t="n">
-        <v>-0.022675252016477344</v>
+      <c r="D66" t="n">
+        <v>-4.122918519774288</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>67</v>
-      </c>
-      <c r="B67" t="n">
+        <v>68</v>
+      </c>
+      <c r="B67" t="n" s="2">
+        <v>40269.0</v>
+      </c>
+      <c r="C67" t="n">
         <v>-0.010319366928693174</v>
       </c>
-      <c r="C67" t="n">
-        <v>-0.01907877574471098</v>
+      <c r="D67" t="n">
+        <v>-3.999484542241838</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>68</v>
-      </c>
-      <c r="B68" t="n">
+        <v>69</v>
+      </c>
+      <c r="B68" t="n" s="2">
+        <v>40360.0</v>
+      </c>
+      <c r="C68" t="n">
         <v>0.01454846275234023</v>
       </c>
-      <c r="C68" t="n">
-        <v>-0.015600614300476795</v>
+      <c r="D68" t="n">
+        <v>-3.844116756246052</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>69</v>
-      </c>
-      <c r="B69" t="n">
+        <v>70</v>
+      </c>
+      <c r="B69" t="n" s="2">
+        <v>40452.0</v>
+      </c>
+      <c r="C69" t="n">
         <v>-0.013412985000381683</v>
       </c>
-      <c r="C69" t="n">
-        <v>-0.012446433926879743</v>
+      <c r="D69" t="n">
+        <v>-3.6773694947187963</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" t="n">
+        <v>71</v>
+      </c>
+      <c r="B70" t="n" s="2">
+        <v>40544.0</v>
+      </c>
+      <c r="C70" t="n">
         <v>-0.0350855251336718</v>
       </c>
-      <c r="C70" t="n">
-        <v>-0.009846788829535272</v>
+      <c r="D70" t="n">
+        <v>-3.523260925236116</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>71</v>
-      </c>
-      <c r="B71" t="n">
+        <v>72</v>
+      </c>
+      <c r="B71" t="n" s="2">
+        <v>40634.0</v>
+      </c>
+      <c r="C71" t="n">
         <v>-0.03505086031570859</v>
       </c>
-      <c r="C71" t="n">
-        <v>-0.009516071194964112</v>
+      <c r="D71" t="n">
+        <v>-3.55497091558572</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>72</v>
-      </c>
-      <c r="B72" t="n">
+        <v>73</v>
+      </c>
+      <c r="B72" t="n" s="2">
+        <v>40725.0</v>
+      </c>
+      <c r="C72" t="n">
         <v>0.01379741255212874</v>
       </c>
-      <c r="C72" t="n">
-        <v>0.0012391625371861552</v>
+      <c r="D72" t="n">
+        <v>-2.5055111831690624</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>73</v>
-      </c>
-      <c r="B73" t="n">
+        <v>74</v>
+      </c>
+      <c r="B73" t="n" s="2">
+        <v>40817.0</v>
+      </c>
+      <c r="C73" t="n">
         <v>0.0897352950693957</v>
       </c>
-      <c r="C73" t="n">
-        <v>0.001959203025106958</v>
+      <c r="D73" t="n">
+        <v>-2.423803490054155</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>74</v>
-      </c>
-      <c r="B74" t="n">
+        <v>75</v>
+      </c>
+      <c r="B74" t="n" s="2">
+        <v>40909.0</v>
+      </c>
+      <c r="C74" t="n">
         <v>0.02855361207777074</v>
       </c>
-      <c r="C74" t="n">
-        <v>0.001030076484466718</v>
+      <c r="D74" t="n">
+        <v>-2.4741185949020306</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>75</v>
-      </c>
-      <c r="B75" t="n">
+        <v>76</v>
+      </c>
+      <c r="B75" t="n" s="2">
+        <v>41000.0</v>
+      </c>
+      <c r="C75" t="n">
         <v>0.07519103813977268</v>
       </c>
-      <c r="C75" t="n">
-        <v>0.0032514993785380357</v>
+      <c r="D75" t="n">
+        <v>-2.179235781424893</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>76</v>
-      </c>
-      <c r="B76" t="n">
+        <v>77</v>
+      </c>
+      <c r="B76" t="n" s="2">
+        <v>41091.0</v>
+      </c>
+      <c r="C76" t="n">
         <v>0.03402034227062334</v>
       </c>
-      <c r="C76" t="n">
-        <v>0.003006264526297063</v>
+      <c r="D76" t="n">
+        <v>-2.1035623179836094</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>77</v>
-      </c>
-      <c r="B77" t="n">
+        <v>78</v>
+      </c>
+      <c r="B77" t="n" s="2">
+        <v>41183.0</v>
+      </c>
+      <c r="C77" t="n">
         <v>0.011824353889619443</v>
       </c>
-      <c r="C77" t="n">
-        <v>0.005312113746569567</v>
+      <c r="D77" t="n">
+        <v>-1.747807354243669</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>78</v>
-      </c>
-      <c r="B78" t="n">
+        <v>79</v>
+      </c>
+      <c r="B78" t="n" s="2">
+        <v>41275.0</v>
+      </c>
+      <c r="C78" t="n">
         <v>-0.021115887076244677</v>
       </c>
-      <c r="C78" t="n">
-        <v>0.003449735594456731</v>
+      <c r="D78" t="n">
+        <v>-1.7861974747093612</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>79</v>
-      </c>
-      <c r="B79" t="n">
+        <v>80</v>
+      </c>
+      <c r="B79" t="n" s="2">
+        <v>41365.0</v>
+      </c>
+      <c r="C79" t="n">
         <v>-0.039823767438954216</v>
       </c>
-      <c r="C79" t="n">
-        <v>-0.0052910866014467366</v>
+      <c r="D79" t="n">
+        <v>-2.4917177794270273</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>80</v>
-      </c>
-      <c r="B80" t="n">
+        <v>81</v>
+      </c>
+      <c r="B80" t="n" s="2">
+        <v>41456.0</v>
+      </c>
+      <c r="C80" t="n">
         <v>-0.006644507460875526</v>
       </c>
-      <c r="C80" t="n">
-        <v>-0.0028435698832595356</v>
+      <c r="D80" t="n">
+        <v>-2.0594377970397204</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>81</v>
-      </c>
-      <c r="B81" t="n">
+        <v>82</v>
+      </c>
+      <c r="B81" t="n" s="2">
+        <v>41548.0</v>
+      </c>
+      <c r="C81" t="n">
         <v>-0.008983174643108383</v>
       </c>
-      <c r="C81" t="n">
-        <v>-0.004422677385108073</v>
+      <c r="D81" t="n">
+        <v>-2.01293235830331</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>82</v>
-      </c>
-      <c r="B82" t="n">
+        <v>83</v>
+      </c>
+      <c r="B82" t="n" s="2">
+        <v>41640.0</v>
+      </c>
+      <c r="C82" t="n">
         <v>-0.010349817659600746</v>
       </c>
-      <c r="C82" t="n">
-        <v>-0.005358439399006125</v>
+      <c r="D82" t="n">
+        <v>-1.8874607328807969</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>83</v>
-      </c>
-      <c r="B83" t="n">
+        <v>84</v>
+      </c>
+      <c r="B83" t="n" s="2">
+        <v>41730.0</v>
+      </c>
+      <c r="C83" t="n">
         <v>-0.018354517425329675</v>
       </c>
-      <c r="C83" t="n">
-        <v>-0.0030652944373412306</v>
+      <c r="D83" t="n">
+        <v>-1.4269994298084399</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>84</v>
-      </c>
-      <c r="B84" t="n">
+        <v>85</v>
+      </c>
+      <c r="B84" t="n" s="2">
+        <v>41821.0</v>
+      </c>
+      <c r="C84" t="n">
         <v>-0.01693692886474707</v>
       </c>
-      <c r="C84" t="n">
-        <v>-0.007660582019971071</v>
+      <c r="D84" t="n">
+        <v>-1.6461499613326325</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>85</v>
-      </c>
-      <c r="B85" t="n">
+        <v>86</v>
+      </c>
+      <c r="B85" t="n" s="2">
+        <v>41913.0</v>
+      </c>
+      <c r="C85" t="n">
         <v>-9.845007137035955E-4</v>
       </c>
-      <c r="C85" t="n">
-        <v>-0.007378895632162023</v>
+      <c r="D85" t="n">
+        <v>-1.3714308171422829</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>86</v>
-      </c>
-      <c r="B86" t="n">
+        <v>87</v>
+      </c>
+      <c r="B86" t="n" s="2">
+        <v>42005.0</v>
+      </c>
+      <c r="C86" t="n">
         <v>0.04322623378512902</v>
       </c>
-      <c r="C86" t="n">
-        <v>-0.01069084992680148</v>
+      <c r="D86" t="n">
+        <v>-1.4534413900653576</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>87</v>
-      </c>
-      <c r="B87" t="n">
+        <v>88</v>
+      </c>
+      <c r="B87" t="n" s="2">
+        <v>42095.0</v>
+      </c>
+      <c r="C87" t="n">
         <v>0.0804928206760247</v>
       </c>
-      <c r="C87" t="n">
-        <v>-0.007045725717791146</v>
+      <c r="D87" t="n">
+        <v>-0.8411088700075453</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>88</v>
-      </c>
-      <c r="B88" t="n">
+        <v>89</v>
+      </c>
+      <c r="B88" t="n" s="2">
+        <v>42186.0</v>
+      </c>
+      <c r="C88" t="n">
         <v>0.14319424309854578</v>
       </c>
-      <c r="C88" t="n">
-        <v>-0.001981616596913663</v>
+      <c r="D88" t="n">
+        <v>-0.09290990278376654</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>89</v>
-      </c>
-      <c r="B89" t="n">
+        <v>90</v>
+      </c>
+      <c r="B89" t="n" s="2">
+        <v>42278.0</v>
+      </c>
+      <c r="C89" t="n">
         <v>0.13969470606752754</v>
       </c>
-      <c r="C89" t="n">
-        <v>-0.00865427222219114</v>
+      <c r="D89" t="n">
+        <v>-0.5295270986895417</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>90</v>
-      </c>
-      <c r="B90" t="n">
+        <v>91</v>
+      </c>
+      <c r="B90" t="n" s="2">
+        <v>42370.0</v>
+      </c>
+      <c r="C90" t="n">
         <v>0.20982319486892997</v>
       </c>
-      <c r="C90" t="n">
-        <v>-0.006880366372615052</v>
+      <c r="D90" t="n">
+        <v>-0.13785933115535443</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>91</v>
-      </c>
-      <c r="B91" t="n">
+        <v>92</v>
+      </c>
+      <c r="B91" t="n" s="2">
+        <v>42461.0</v>
+      </c>
+      <c r="C91" t="n">
         <v>0.24219006807397525</v>
       </c>
-      <c r="C91" t="n">
-        <v>-0.005858945476808642</v>
+      <c r="D91" t="n">
+        <v>0.15641636941197135</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>92</v>
-      </c>
-      <c r="B92" t="n">
+        <v>93</v>
+      </c>
+      <c r="B92" t="n" s="2">
+        <v>42552.0</v>
+      </c>
+      <c r="C92" t="n">
         <v>0.28140959644665786</v>
       </c>
-      <c r="C92" t="n">
-        <v>0.001519548080138565</v>
+      <c r="D92" t="n">
+        <v>1.058053354059929</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>93</v>
-      </c>
-      <c r="B93" t="n">
+        <v>94</v>
+      </c>
+      <c r="B93" t="n" s="2">
+        <v>42644.0</v>
+      </c>
+      <c r="C93" t="n">
         <v>0.31802238277495065</v>
       </c>
-      <c r="C93" t="n">
-        <v>0.008553640865933444</v>
+      <c r="D93" t="n">
+        <v>1.8903356850241693</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>94</v>
-      </c>
-      <c r="B94" t="n">
+        <v>95</v>
+      </c>
+      <c r="B94" t="n" s="2">
+        <v>42736.0</v>
+      </c>
+      <c r="C94" t="n">
         <v>0.31899780438799885</v>
       </c>
-      <c r="C94" t="n">
-        <v>0.01245552659391077</v>
+      <c r="D94" t="n">
+        <v>2.3680091108575496</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>95</v>
-      </c>
-      <c r="B95" t="n">
+        <v>96</v>
+      </c>
+      <c r="B95" t="n" s="2">
+        <v>42826.0</v>
+      </c>
+      <c r="C95" t="n">
         <v>0.20952915166667707</v>
       </c>
-      <c r="C95" t="n">
-        <v>0.015323454297968067</v>
+      <c r="D95" t="n">
+        <v>2.694959514723294</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>96</v>
-      </c>
-      <c r="B96" t="n">
+        <v>97</v>
+      </c>
+      <c r="B96" t="n" s="2">
+        <v>42917.0</v>
+      </c>
+      <c r="C96" t="n">
         <v>0.17144082834229546</v>
       </c>
-      <c r="C96" t="n">
-        <v>0.012743585745184603</v>
+      <c r="D96" t="n">
+        <v>2.42464252351553</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>97</v>
-      </c>
-      <c r="B97" t="n">
+        <v>98</v>
+      </c>
+      <c r="B97" t="n" s="2">
+        <v>43009.0</v>
+      </c>
+      <c r="C97" t="n">
         <v>0.22942026896407608</v>
       </c>
-      <c r="C97" t="n">
-        <v>0.02082358702841583</v>
+      <c r="D97" t="n">
+        <v>3.163621912598913</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>98</v>
-      </c>
-      <c r="B98" t="n">
+        <v>99</v>
+      </c>
+      <c r="B98" t="n" s="2">
+        <v>43101.0</v>
+      </c>
+      <c r="C98" t="n">
         <v>0.22417450379630988</v>
       </c>
-      <c r="C98" t="n">
-        <v>0.02775667793662416</v>
+      <c r="D98" t="n">
+        <v>3.727813301058447</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>99</v>
-      </c>
-      <c r="B99" t="n">
+        <v>100</v>
+      </c>
+      <c r="B99" t="n" s="2">
+        <v>43191.0</v>
+      </c>
+      <c r="C99" t="n">
         <v>0.26547364058008993</v>
       </c>
-      <c r="C99" t="n">
-        <v>0.0266285880918829</v>
+      <c r="D99" t="n">
+        <v>3.423684765478896</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>100</v>
-      </c>
-      <c r="B100" t="n">
+        <v>101</v>
+      </c>
+      <c r="B100" t="n" s="2">
+        <v>43282.0</v>
+      </c>
+      <c r="C100" t="n">
         <v>0.2030070130967585</v>
       </c>
-      <c r="C100" t="n">
-        <v>0.030706333932839502</v>
+      <c r="D100" t="n">
+        <v>3.5775678564741398</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>101</v>
-      </c>
-      <c r="B101" t="n">
+        <v>102</v>
+      </c>
+      <c r="B101" t="n" s="2">
+        <v>43374.0</v>
+      </c>
+      <c r="C101" t="n">
         <v>0.22897010696507536</v>
       </c>
-      <c r="C101" t="n">
-        <v>0.026851827531437257</v>
+      <c r="D101" t="n">
+        <v>2.876947974742805</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>102</v>
-      </c>
-      <c r="B102" t="n">
+        <v>103</v>
+      </c>
+      <c r="B102" t="n" s="2">
+        <v>43466.0</v>
+      </c>
+      <c r="C102" t="n">
         <v>0.18846370343198138</v>
       </c>
-      <c r="C102" t="n">
-        <v>0.027431732507384766</v>
+      <c r="D102" t="n">
+        <v>2.5617048216313165</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>103</v>
-      </c>
-      <c r="B103" t="n">
+        <v>104</v>
+      </c>
+      <c r="B103" t="n" s="2">
+        <v>43556.0</v>
+      </c>
+      <c r="C103" t="n">
         <v>0.18841086363473125</v>
       </c>
-      <c r="C103" t="n">
-        <v>0.02529409362968891</v>
+      <c r="D103" t="n">
+        <v>1.9215344526362088</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>104</v>
-      </c>
-      <c r="B104" t="n">
+        <v>105</v>
+      </c>
+      <c r="B104" t="n" s="2">
+        <v>43647.0</v>
+      </c>
+      <c r="C104" t="n">
         <v>0.19965826386583796</v>
       </c>
-      <c r="C104" t="n">
-        <v>0.03070603732024616</v>
+      <c r="D104" t="n">
+        <v>1.9897555718252136</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>105</v>
-      </c>
-      <c r="B105" t="n">
+        <v>106</v>
+      </c>
+      <c r="B105" t="n" s="2">
+        <v>43739.0</v>
+      </c>
+      <c r="C105" t="n">
         <v>0.17742915527932746</v>
       </c>
-      <c r="C105" t="n">
-        <v>0.020121660359607954</v>
+      <c r="D105" t="n">
+        <v>0.419964799982786</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>106</v>
-      </c>
-      <c r="B106" t="n">
+        <v>107</v>
+      </c>
+      <c r="B106" t="n" s="2">
+        <v>43831.0</v>
+      </c>
+      <c r="C106" t="n">
         <v>0.20866354464976244</v>
       </c>
-      <c r="C106" t="n">
-        <v>0.013047185592468351</v>
+      <c r="D106" t="n">
+        <v>-0.8271095083591362</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>107</v>
-      </c>
-      <c r="B107" t="n">
+        <v>108</v>
+      </c>
+      <c r="B107" t="n" s="2">
+        <v>43922.0</v>
+      </c>
+      <c r="C107" t="n">
         <v>0.39612830772594565</v>
       </c>
-      <c r="C107" t="n">
-        <v>-0.1366308815817851</v>
+      <c r="D107" t="n">
+        <v>-16.35145313942754</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>108</v>
-      </c>
-      <c r="B108" t="n">
+        <v>109</v>
+      </c>
+      <c r="B108" t="n" s="2">
+        <v>44013.0</v>
+      </c>
+      <c r="C108" t="n">
         <v>0.3324660946921987</v>
       </c>
-      <c r="C108" t="n">
-        <v>-0.040774825437239676</v>
+      <c r="D108" t="n">
+        <v>-7.3271153976966374</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>109</v>
-      </c>
-      <c r="B109" t="n">
+        <v>110</v>
+      </c>
+      <c r="B109" t="n" s="2">
+        <v>44105.0</v>
+      </c>
+      <c r="C109" t="n">
         <v>0.24476842248683983</v>
       </c>
-      <c r="C109" t="n">
-        <v>-0.017460259927528334</v>
+      <c r="D109" t="n">
+        <v>-5.558017985694796</v>
       </c>
     </row>
   </sheetData>

</xml_diff>